<commit_message>
Changed orthographical representations to IPA
</commit_message>
<xml_diff>
--- a/tutorial/turkish-vowels.xlsx
+++ b/tutorial/turkish-vowels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicagank/Desktop/VowSpace/VowSpace/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAF0DE0-9617-9A4D-B5E1-4DA874A2E8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E11D66B-8B44-334E-9090-51AAD989542E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,16 +47,10 @@
     <t>/e/</t>
   </si>
   <si>
-    <t>/ı/</t>
-  </si>
-  <si>
     <t>/i/</t>
   </si>
   <si>
     <t>/o/</t>
-  </si>
-  <si>
-    <t>/ö/</t>
   </si>
   <si>
     <t>Türkçe</t>
@@ -65,13 +59,19 @@
     <t>/u/</t>
   </si>
   <si>
-    <t>/ü/</t>
-  </si>
-  <si>
     <t>f1</t>
   </si>
   <si>
     <t>f2</t>
+  </si>
+  <si>
+    <t>/ɯ/</t>
+  </si>
+  <si>
+    <t>/œ/</t>
+  </si>
+  <si>
+    <t>/y/</t>
   </si>
 </sst>
 </file>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -472,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -492,7 +492,7 @@
         <v>1125</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -506,7 +506,7 @@
         <v>1036</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -520,7 +520,7 @@
         <v>1177</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -534,7 +534,7 @@
         <v>1060</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>1210</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -562,7 +562,7 @@
         <v>1201</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -576,7 +576,7 @@
         <v>1845</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -590,7 +590,7 @@
         <v>1750</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -604,7 +604,7 @@
         <v>1861</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>1780</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -632,7 +632,7 @@
         <v>1704</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -646,12 +646,12 @@
         <v>1768</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2">
         <v>438</v>
@@ -660,12 +660,12 @@
         <v>1427</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
         <v>417</v>
@@ -674,12 +674,12 @@
         <v>1434</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B16" s="2">
         <v>432</v>
@@ -688,12 +688,12 @@
         <v>1460</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B17" s="2">
         <v>394</v>
@@ -702,12 +702,12 @@
         <v>1675</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B18" s="2">
         <v>428</v>
@@ -716,12 +716,12 @@
         <v>1501</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B19" s="2">
         <v>399</v>
@@ -730,12 +730,12 @@
         <v>1544</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3">
         <v>314</v>
@@ -744,12 +744,12 @@
         <v>2070</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3">
         <v>297</v>
@@ -758,12 +758,12 @@
         <v>2084</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3">
         <v>318</v>
@@ -772,12 +772,12 @@
         <v>2049</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="3">
         <v>294</v>
@@ -786,12 +786,12 @@
         <v>2091</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3">
         <v>352</v>
@@ -800,12 +800,12 @@
         <v>2077</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="3">
         <v>303</v>
@@ -814,12 +814,12 @@
         <v>2080</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" s="3">
         <v>499</v>
@@ -828,12 +828,12 @@
         <v>841</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27" s="3">
         <v>485</v>
@@ -842,12 +842,12 @@
         <v>826</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="3">
         <v>520</v>
@@ -856,12 +856,12 @@
         <v>889</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" s="3">
         <v>500</v>
@@ -870,12 +870,12 @@
         <v>897</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" s="3">
         <v>508</v>
@@ -884,12 +884,12 @@
         <v>844</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="3">
         <v>492</v>
@@ -898,12 +898,12 @@
         <v>884</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B32" s="3">
         <v>462</v>
@@ -912,12 +912,12 @@
         <v>1434</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B33" s="3">
         <v>477</v>
@@ -926,12 +926,12 @@
         <v>1387</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B34" s="3">
         <v>496</v>
@@ -940,12 +940,12 @@
         <v>1333</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B35" s="3">
         <v>451</v>
@@ -954,12 +954,12 @@
         <v>1539</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B36" s="3">
         <v>469</v>
@@ -968,12 +968,12 @@
         <v>1465</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B37" s="3">
         <v>481</v>
@@ -982,12 +982,12 @@
         <v>1428</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B38" s="3">
         <v>413</v>
@@ -996,12 +996,12 @@
         <v>895</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="3">
         <v>391</v>
@@ -1010,12 +1010,12 @@
         <v>832</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B40" s="3">
         <v>392</v>
@@ -1024,12 +1024,12 @@
         <v>982</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B41" s="3">
         <v>378</v>
@@ -1038,12 +1038,12 @@
         <v>985</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="3">
         <v>385</v>
@@ -1052,12 +1052,12 @@
         <v>875</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B43" s="3">
         <v>374</v>
@@ -1066,12 +1066,12 @@
         <v>968</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B44" s="3">
         <v>370</v>
@@ -1080,12 +1080,12 @@
         <v>1622</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B45" s="3">
         <v>315</v>
@@ -1094,12 +1094,12 @@
         <v>1772</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B46" s="3">
         <v>340</v>
@@ -1108,12 +1108,12 @@
         <v>1714</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B47" s="3">
         <v>313</v>
@@ -1122,12 +1122,12 @@
         <v>1701</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B48" s="3">
         <v>335</v>
@@ -1136,12 +1136,12 @@
         <v>1752</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B49" s="3">
         <v>301</v>
@@ -1150,7 +1150,7 @@
         <v>1829</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>